<commit_message>
added multiple batch mapping to fas
</commit_message>
<xml_diff>
--- a/src/excel-templates/add-students.xlsx
+++ b/src/excel-templates/add-students.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahna\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6759BE9F-4B25-4DCD-AF84-7CC7E6C2A486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5512383B-7944-4704-9A3C-ED2A79B6DE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="990" windowWidth="15135" windowHeight="9525" xr2:uid="{E7F23789-AB23-4973-B0CB-F700D0BC59A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E7F23789-AB23-4973-B0CB-F700D0BC59A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="CINTEL">Sheet1!$J$2:$J$8</definedName>
-    <definedName name="CTECH">Sheet1!$L$2</definedName>
-    <definedName name="DSBS">Sheet1!$K$2:$K$7</definedName>
-    <definedName name="NWC">Sheet1!$M$2:$M$10</definedName>
+    <definedName name="CINTEL">Sheet2!$A$2:$A$8</definedName>
+    <definedName name="CTECH">Sheet2!$C$2</definedName>
+    <definedName name="DSBS">Sheet2!$B$2:$B$7</definedName>
+    <definedName name="NWC">Sheet2!$D$2:$D$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Registration Number</t>
   </si>
@@ -133,13 +134,28 @@
   </si>
   <si>
     <t>M.Tech (Integrated) - Cyber Security and Digital  Forensics</t>
+  </si>
+  <si>
+    <t>DSBS</t>
+  </si>
+  <si>
+    <t>Career Option</t>
+  </si>
+  <si>
+    <t>Superset Enrolled</t>
+  </si>
+  <si>
+    <t>Higher Studies</t>
+  </si>
+  <si>
+    <t>Entrepreneur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +166,24 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -175,9 +209,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,7 +531,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,127 +574,33 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -669,14 +611,166 @@
       <c r="N11" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{1888002C-8B94-456C-9A40-DB219B78434E}">
-      <formula1>$J$1:$M$1</formula1>
-    </dataValidation>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{26ABA371-C8DE-402E-A364-88AFE50F7700}">
       <formula1>INDIRECT($D$2)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1888002C-8B94-456C-9A40-DB219B78434E}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$1:$D$1</xm:f>
+          </x14:formula1>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9CB37A2F-35FB-407C-849D-849F8A850EB4}">
+          <x14:formula1>
+            <xm:f>Sheet2!$E$2:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>G1:G1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA9DA25-6674-4F2D-9732-EEB878EA03FF}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="82.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" customWidth="1"/>
+    <col min="4" max="4" width="74.42578125" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed companies missing bug, updated placement %
</commit_message>
<xml_diff>
--- a/src/excel-templates/add-students.xlsx
+++ b/src/excel-templates/add-students.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahna\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahna\Desktop\placement-details\placement-details\src\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5512383B-7944-4704-9A3C-ED2A79B6DE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC1C30B-3783-4710-BC80-F23BB0F8A0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E7F23789-AB23-4973-B0CB-F700D0BC59A0}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Registration Number</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Entrepreneur</t>
+  </si>
+  <si>
+    <t>Arrear/Detained</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +632,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9CB37A2F-35FB-407C-849D-849F8A850EB4}">
           <x14:formula1>
-            <xm:f>Sheet2!$E$2:$E$4</xm:f>
+            <xm:f>Sheet2!$E$1:$E$5</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
@@ -644,7 +647,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,6 +731,9 @@
       <c r="D5" t="s">
         <v>28</v>
       </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">

</xml_diff>